<commit_message>
2nd fb tone added
</commit_message>
<xml_diff>
--- a/translations/translation_eng.xlsx
+++ b/translations/translation_eng.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29530"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pcadmin\Documents\dok\TARU\PROJEKTID\EEGManyLabs\Task\spotlight_replication\translations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F678F1A5-BF66-4BB2-B44E-0EBF884EBB05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{364BFF60-3C09-4B07-983B-99E1A250580F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
   <si>
     <t>key</t>
   </si>
@@ -123,11 +123,19 @@
     <t>Please fixate on the dot below...</t>
   </si>
   <si>
-    <t>Before starting the main experiment, you will have the opportunity to practice during 4 shorter blocks. These practice blocks are designed to help you get familiar with the task.\n\n
-During practice trials:\n- A feedback tone will play whenever you correctly press the spacebar in response to a pair of eights appearing at the attended locations.\n-You are encouraged to ask the experimenter any questions either now or during the practice trials.\n</t>
-  </si>
-  <si>
     <t>You will briefly see eye-movement calibration screens before the practice trials and occasionally throughout the experiment. Simply look at the dot when it appears and follow it with your eyes as it changes position. Please try to keep your head still and avoid blinking when possible.\n\nPress "space" to begin with the practice…</t>
+  </si>
+  <si>
+    <t>Before starting the main experiment, you will have the opportunity to practice during 4 shorter blocks. These practice blocks are designed to help you get familiar with the task.</t>
+  </si>
+  <si>
+    <t>general_intro_5</t>
+  </si>
+  <si>
+    <t>During practice trials:\n
+- A feedback tone will play whenever you correctly press the spacebar in response to a pair of eights appearing at the attended locations.
+-  To facilitate training, an additional lower-pitched tone will play whenever a pair appears, but only during the first half of the block (before the hand switch).
+- You are encouraged to ask the experimenter any questions either now or during the practice trials.</t>
   </si>
 </sst>
 </file>
@@ -448,10 +456,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B14"/>
+  <dimension ref="A1:B15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -497,78 +505,86 @@
         <v>24</v>
       </c>
       <c r="B5" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="114.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>28</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>2</v>
+      </c>
+      <c r="B7" s="1" t="s">
         <v>26</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>2</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>3</v>
-      </c>
-      <c r="B7" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B8" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B9" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>20</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>21</v>
+        <v>5</v>
+      </c>
+      <c r="B10" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>6</v>
-      </c>
-      <c r="B11" t="s">
-        <v>12</v>
+        <v>20</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B12" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B13" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
+        <v>8</v>
+      </c>
+      <c r="B14" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
         <v>22</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B15" t="s">
         <v>25</v>
       </c>
     </row>

</xml_diff>